<commit_message>
added Dockerfile and requirements.txt
</commit_message>
<xml_diff>
--- a/domain_expiry_date.xlsx
+++ b/domain_expiry_date.xlsx
@@ -14,30 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Домен</t>
   </si>
   <si>
     <t>Дата окончания</t>
-  </si>
-  <si>
-    <t>spiritofhelsinki.com</t>
-  </si>
-  <si>
-    <t>Узнать дату окончания не получилось (Вероятно домен свободен)</t>
-  </si>
-  <si>
-    <t>tkstkdsoft.com</t>
-  </si>
-  <si>
-    <t>30.04.2024</t>
-  </si>
-  <si>
-    <t>voteexpress.com</t>
-  </si>
-  <si>
-    <t>01.07.2024</t>
   </si>
   <si>
     <t>vk.com</t>
@@ -67,18 +49,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,10 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,14 +366,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="62.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -410,35 +385,11 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>